<commit_message>
fixed base spd of spectra
</commit_message>
<xml_diff>
--- a/output/xlsx_reports/speed_charts.xlsx
+++ b/output/xlsx_reports/speed_charts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuzzy\BKsDBTools\summoners_war_0_1_0\output\xlsx_reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuzzy\bk_sw_tools_DEV\output\xlsx_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -860,27 +860,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -894,6 +873,27 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1189,7 +1189,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1201,7 +1201,7 @@
     <col min="5" max="5" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.81640625" customWidth="1"/>
     <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" style="107" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" style="100" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="5.81640625" customWidth="1"/>
     <col min="11" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
@@ -1218,7 +1218,7 @@
       <c r="E1" s="69"/>
       <c r="F1" s="69"/>
       <c r="G1" s="67"/>
-      <c r="H1" s="103"/>
+      <c r="H1" s="96"/>
       <c r="I1" s="70"/>
       <c r="J1" s="50" t="s">
         <v>27</v>
@@ -1226,10 +1226,10 @@
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
       <c r="R1" s="10"/>
       <c r="S1" s="10"/>
       <c r="T1" s="10"/>
@@ -1245,14 +1245,14 @@
       <c r="D2" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="97" t="s">
+      <c r="E2" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="97"/>
+      <c r="F2" s="106"/>
       <c r="G2" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="104" t="s">
+      <c r="H2" s="97" t="s">
         <v>52</v>
       </c>
       <c r="I2" s="71" t="s">
@@ -1262,12 +1262,12 @@
       <c r="K2" s="87"/>
       <c r="L2" s="87"/>
       <c r="M2" s="87"/>
-      <c r="N2" s="99" t="s">
+      <c r="N2" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="101"/>
+      <c r="O2" s="108"/>
+      <c r="P2" s="108"/>
+      <c r="Q2" s="109"/>
       <c r="R2" s="87"/>
       <c r="S2" s="87"/>
       <c r="T2" s="87"/>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="D3" s="82"/>
       <c r="E3" s="83">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="F3" s="84">
         <v>0.15</v>
@@ -1343,66 +1343,66 @@
       <c r="D4" s="95">
         <v>102</v>
       </c>
-      <c r="E4" s="98">
+      <c r="E4" s="103">
         <f>SUM($D4*(1+$E$3+$F$3))</f>
-        <v>117.3</v>
-      </c>
-      <c r="F4" s="98"/>
+        <v>141.78</v>
+      </c>
+      <c r="F4" s="103"/>
       <c r="G4" s="89">
         <v>38</v>
       </c>
-      <c r="H4" s="105">
+      <c r="H4" s="98">
         <f>SUM($H$3)</f>
         <v>0.33</v>
       </c>
       <c r="I4" s="73">
         <f>SUM(($E4+$G4)*(1+$H4))</f>
-        <v>206.54900000000004</v>
+        <v>239.10740000000001</v>
       </c>
       <c r="J4" s="53"/>
       <c r="K4" s="53">
         <f>SUM($I4*(0.07*1))</f>
-        <v>14.458430000000003</v>
+        <v>16.737518000000001</v>
       </c>
       <c r="L4" s="53">
         <f>SUM($I4*(0.07*2))</f>
-        <v>28.916860000000007</v>
+        <v>33.475036000000003</v>
       </c>
       <c r="M4" s="53">
         <f>SUM($I4*(0.07*3))</f>
-        <v>43.375290000000014</v>
+        <v>50.212554000000004</v>
       </c>
       <c r="N4" s="53">
         <f>SUM($I4*(0.07*4))</f>
-        <v>57.833720000000014</v>
+        <v>66.950072000000006</v>
       </c>
       <c r="O4" s="53">
         <f>SUM($I4*(0.07*5))</f>
-        <v>72.292150000000021</v>
+        <v>83.687590000000014</v>
       </c>
       <c r="P4" s="53">
         <f>SUM($I4*(0.07*6))</f>
-        <v>86.750580000000028</v>
+        <v>100.42510800000001</v>
       </c>
       <c r="Q4" s="53">
         <f>SUM($I4*(0.07*7))</f>
-        <v>101.20901000000002</v>
+        <v>117.16262600000002</v>
       </c>
       <c r="R4" s="53">
         <f>SUM($I4*(0.07*8))</f>
-        <v>115.66744000000003</v>
+        <v>133.90014400000001</v>
       </c>
       <c r="S4" s="53">
         <f>SUM($I4*(0.07*9))</f>
-        <v>130.12587000000005</v>
+        <v>150.63766200000003</v>
       </c>
       <c r="T4" s="53">
         <f>SUM($I4*(0.07*10))</f>
-        <v>144.58430000000004</v>
+        <v>167.37518000000003</v>
       </c>
       <c r="U4" s="54">
         <f>SUM($I4*(0.07*11))</f>
-        <v>159.04273000000003</v>
+        <v>184.11269800000002</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
@@ -1414,68 +1414,68 @@
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="64">
-        <v>116</v>
-      </c>
-      <c r="E5" s="98">
+        <v>126</v>
+      </c>
+      <c r="E5" s="103">
         <f>SUM($D5*(1+$E$3+$F$3))</f>
-        <v>133.39999999999998</v>
-      </c>
-      <c r="F5" s="98"/>
+        <v>175.14</v>
+      </c>
+      <c r="F5" s="103"/>
       <c r="G5" s="89">
         <v>20</v>
       </c>
-      <c r="H5" s="105">
+      <c r="H5" s="98">
         <f t="shared" ref="H5:H21" si="0">SUM($H$3)</f>
         <v>0.33</v>
       </c>
       <c r="I5" s="73">
         <f>SUM(($E5+$G5)*(1+$H5))</f>
-        <v>204.02199999999999</v>
+        <v>259.53620000000001</v>
       </c>
       <c r="J5" s="53"/>
       <c r="K5" s="53">
         <f t="shared" ref="K5:K21" si="1">SUM($I5*(0.07*1))</f>
-        <v>14.281540000000001</v>
+        <v>18.167534000000003</v>
       </c>
       <c r="L5" s="53">
         <f t="shared" ref="L5:L21" si="2">SUM($I5*(0.07*2))</f>
-        <v>28.563080000000003</v>
+        <v>36.335068000000007</v>
       </c>
       <c r="M5" s="53">
         <f t="shared" ref="M5:M21" si="3">SUM($I5*(0.07*3))</f>
-        <v>42.844619999999999</v>
+        <v>54.50260200000001</v>
       </c>
       <c r="N5" s="53">
         <f t="shared" ref="N5:N21" si="4">SUM($I5*(0.07*4))</f>
-        <v>57.126160000000006</v>
+        <v>72.670136000000014</v>
       </c>
       <c r="O5" s="53">
         <f t="shared" ref="O5:O21" si="5">SUM($I5*(0.07*5))</f>
-        <v>71.407700000000006</v>
+        <v>90.837670000000017</v>
       </c>
       <c r="P5" s="53">
         <f t="shared" ref="P5:P21" si="6">SUM($I5*(0.07*6))</f>
-        <v>85.689239999999998</v>
+        <v>109.00520400000002</v>
       </c>
       <c r="Q5" s="53">
         <f t="shared" ref="Q5:Q21" si="7">SUM($I5*(0.07*7))</f>
-        <v>99.970780000000005</v>
+        <v>127.17273800000001</v>
       </c>
       <c r="R5" s="53">
         <f t="shared" ref="R5:R21" si="8">SUM($I5*(0.07*8))</f>
-        <v>114.25232000000001</v>
+        <v>145.34027200000003</v>
       </c>
       <c r="S5" s="53">
         <f t="shared" ref="S5:S21" si="9">SUM($I5*(0.07*9))</f>
-        <v>128.53386</v>
+        <v>163.50780600000004</v>
       </c>
       <c r="T5" s="53">
         <f t="shared" ref="T5:T21" si="10">SUM($I5*(0.07*10))</f>
-        <v>142.81540000000001</v>
+        <v>181.67534000000003</v>
       </c>
       <c r="U5" s="54">
         <f t="shared" ref="U5:U21" si="11">SUM($I5*(0.07*11))</f>
-        <v>157.09693999999999</v>
+        <v>199.84287400000002</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="29" x14ac:dyDescent="0.35">
@@ -1489,66 +1489,66 @@
       <c r="D6" s="63">
         <v>116</v>
       </c>
-      <c r="E6" s="98">
+      <c r="E6" s="103">
         <f t="shared" ref="E6:E21" si="12">SUM($D6*(1+$E$3+$F$3))</f>
-        <v>133.39999999999998</v>
-      </c>
-      <c r="F6" s="98"/>
+        <v>161.23999999999998</v>
+      </c>
+      <c r="F6" s="103"/>
       <c r="G6" s="89">
         <v>156</v>
       </c>
-      <c r="H6" s="105">
+      <c r="H6" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I6" s="73">
         <f t="shared" ref="I6:I21" si="13">SUM(($E6+$G6)*(1+$H6))</f>
-        <v>384.90199999999999</v>
+        <v>421.92920000000004</v>
       </c>
       <c r="J6" s="53"/>
       <c r="K6" s="53">
         <f t="shared" si="1"/>
-        <v>26.943140000000003</v>
+        <v>29.535044000000006</v>
       </c>
       <c r="L6" s="53">
         <f t="shared" si="2"/>
-        <v>53.886280000000006</v>
+        <v>59.070088000000013</v>
       </c>
       <c r="M6" s="53">
         <f t="shared" si="3"/>
-        <v>80.829419999999999</v>
+        <v>88.605132000000012</v>
       </c>
       <c r="N6" s="53">
         <f t="shared" si="4"/>
-        <v>107.77256000000001</v>
+        <v>118.14017600000003</v>
       </c>
       <c r="O6" s="53">
         <f t="shared" si="5"/>
-        <v>134.7157</v>
+        <v>147.67522000000002</v>
       </c>
       <c r="P6" s="53">
         <f t="shared" si="6"/>
-        <v>161.65884</v>
+        <v>177.21026400000002</v>
       </c>
       <c r="Q6" s="53">
         <f t="shared" si="7"/>
-        <v>188.60198</v>
+        <v>206.74530800000005</v>
       </c>
       <c r="R6" s="53">
         <f t="shared" si="8"/>
-        <v>215.54512000000003</v>
+        <v>236.28035200000005</v>
       </c>
       <c r="S6" s="53">
         <f t="shared" si="9"/>
-        <v>242.48826000000003</v>
+        <v>265.81539600000008</v>
       </c>
       <c r="T6" s="53">
         <f t="shared" si="10"/>
-        <v>269.4314</v>
+        <v>295.35044000000005</v>
       </c>
       <c r="U6" s="54">
         <f t="shared" si="11"/>
-        <v>296.37454000000002</v>
+        <v>324.88548400000002</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
@@ -1564,66 +1564,66 @@
       <c r="D7" s="63">
         <v>120</v>
       </c>
-      <c r="E7" s="98">
+      <c r="E7" s="103">
         <f t="shared" si="12"/>
-        <v>138</v>
-      </c>
-      <c r="F7" s="98"/>
+        <v>166.79999999999998</v>
+      </c>
+      <c r="F7" s="103"/>
       <c r="G7" s="89">
         <v>162</v>
       </c>
-      <c r="H7" s="105">
+      <c r="H7" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I7" s="73">
         <f t="shared" si="13"/>
-        <v>399</v>
+        <v>437.30399999999997</v>
       </c>
       <c r="J7" s="53"/>
       <c r="K7" s="53">
         <f t="shared" si="1"/>
-        <v>27.930000000000003</v>
+        <v>30.611280000000001</v>
       </c>
       <c r="L7" s="53">
         <f t="shared" si="2"/>
-        <v>55.860000000000007</v>
+        <v>61.222560000000001</v>
       </c>
       <c r="M7" s="53">
         <f t="shared" si="3"/>
-        <v>83.79</v>
+        <v>91.833840000000009</v>
       </c>
       <c r="N7" s="53">
         <f t="shared" si="4"/>
-        <v>111.72000000000001</v>
+        <v>122.44512</v>
       </c>
       <c r="O7" s="53">
         <f t="shared" si="5"/>
-        <v>139.65</v>
+        <v>153.0564</v>
       </c>
       <c r="P7" s="53">
         <f t="shared" si="6"/>
-        <v>167.58</v>
+        <v>183.66768000000002</v>
       </c>
       <c r="Q7" s="53">
         <f t="shared" si="7"/>
-        <v>195.51000000000002</v>
+        <v>214.27896000000001</v>
       </c>
       <c r="R7" s="53">
         <f t="shared" si="8"/>
-        <v>223.44000000000003</v>
+        <v>244.89024000000001</v>
       </c>
       <c r="S7" s="53">
         <f t="shared" si="9"/>
-        <v>251.37000000000003</v>
+        <v>275.50152000000003</v>
       </c>
       <c r="T7" s="53">
         <f t="shared" si="10"/>
-        <v>279.3</v>
+        <v>306.11279999999999</v>
       </c>
       <c r="U7" s="54">
         <f t="shared" si="11"/>
-        <v>307.23</v>
+        <v>336.72408000000001</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
@@ -1639,66 +1639,66 @@
       <c r="D8" s="63">
         <v>96</v>
       </c>
-      <c r="E8" s="98">
+      <c r="E8" s="103">
         <f t="shared" si="12"/>
-        <v>110.39999999999999</v>
-      </c>
-      <c r="F8" s="98"/>
+        <v>133.44</v>
+      </c>
+      <c r="F8" s="103"/>
       <c r="G8" s="89">
         <v>100</v>
       </c>
-      <c r="H8" s="105">
+      <c r="H8" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I8" s="73">
         <f t="shared" si="13"/>
-        <v>279.83199999999999</v>
+        <v>310.47520000000003</v>
       </c>
       <c r="J8" s="53"/>
       <c r="K8" s="53">
         <f t="shared" si="1"/>
-        <v>19.588240000000003</v>
+        <v>21.733264000000005</v>
       </c>
       <c r="L8" s="53">
         <f t="shared" si="2"/>
-        <v>39.176480000000005</v>
+        <v>43.466528000000011</v>
       </c>
       <c r="M8" s="53">
         <f t="shared" si="3"/>
-        <v>58.764720000000004</v>
+        <v>65.199792000000016</v>
       </c>
       <c r="N8" s="53">
         <f t="shared" si="4"/>
-        <v>78.35296000000001</v>
+        <v>86.933056000000022</v>
       </c>
       <c r="O8" s="53">
         <f t="shared" si="5"/>
-        <v>97.941200000000009</v>
+        <v>108.66632000000003</v>
       </c>
       <c r="P8" s="53">
         <f t="shared" si="6"/>
-        <v>117.52944000000001</v>
+        <v>130.39958400000003</v>
       </c>
       <c r="Q8" s="53">
         <f t="shared" si="7"/>
-        <v>137.11768000000001</v>
+        <v>152.13284800000002</v>
       </c>
       <c r="R8" s="53">
         <f t="shared" si="8"/>
-        <v>156.70592000000002</v>
+        <v>173.86611200000004</v>
       </c>
       <c r="S8" s="53">
         <f t="shared" si="9"/>
-        <v>176.29416000000003</v>
+        <v>195.59937600000006</v>
       </c>
       <c r="T8" s="53">
         <f t="shared" si="10"/>
-        <v>195.88240000000002</v>
+        <v>217.33264000000005</v>
       </c>
       <c r="U8" s="54">
         <f t="shared" si="11"/>
-        <v>215.47064</v>
+        <v>239.06590400000002</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
@@ -1714,66 +1714,66 @@
       <c r="D9" s="63">
         <v>99</v>
       </c>
-      <c r="E9" s="98">
+      <c r="E9" s="103">
         <f t="shared" si="12"/>
-        <v>113.85</v>
-      </c>
-      <c r="F9" s="98"/>
+        <v>137.60999999999999</v>
+      </c>
+      <c r="F9" s="103"/>
       <c r="G9" s="89">
         <v>250</v>
       </c>
-      <c r="H9" s="105">
+      <c r="H9" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I9" s="73">
         <f t="shared" si="13"/>
-        <v>483.92050000000006</v>
+        <v>515.5213</v>
       </c>
       <c r="J9" s="53"/>
       <c r="K9" s="53">
         <f t="shared" si="1"/>
-        <v>33.874435000000005</v>
+        <v>36.086491000000002</v>
       </c>
       <c r="L9" s="53">
         <f t="shared" si="2"/>
-        <v>67.748870000000011</v>
+        <v>72.172982000000005</v>
       </c>
       <c r="M9" s="53">
         <f t="shared" si="3"/>
-        <v>101.62330500000002</v>
+        <v>108.25947300000001</v>
       </c>
       <c r="N9" s="53">
         <f t="shared" si="4"/>
-        <v>135.49774000000002</v>
+        <v>144.34596400000001</v>
       </c>
       <c r="O9" s="53">
         <f t="shared" si="5"/>
-        <v>169.37217500000003</v>
+        <v>180.432455</v>
       </c>
       <c r="P9" s="53">
         <f t="shared" si="6"/>
-        <v>203.24661000000003</v>
+        <v>216.51894600000003</v>
       </c>
       <c r="Q9" s="53">
         <f t="shared" si="7"/>
-        <v>237.12104500000007</v>
+        <v>252.60543700000002</v>
       </c>
       <c r="R9" s="53">
         <f t="shared" si="8"/>
-        <v>270.99548000000004</v>
+        <v>288.69192800000002</v>
       </c>
       <c r="S9" s="53">
         <f t="shared" si="9"/>
-        <v>304.86991500000011</v>
+        <v>324.77841900000004</v>
       </c>
       <c r="T9" s="53">
         <f t="shared" si="10"/>
-        <v>338.74435000000005</v>
+        <v>360.86491000000001</v>
       </c>
       <c r="U9" s="54">
         <f t="shared" si="11"/>
-        <v>372.61878500000006</v>
+        <v>396.95140100000003</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
@@ -1789,66 +1789,66 @@
       <c r="D10" s="63">
         <v>95</v>
       </c>
-      <c r="E10" s="98">
+      <c r="E10" s="103">
         <f t="shared" si="12"/>
-        <v>109.24999999999999</v>
-      </c>
-      <c r="F10" s="98"/>
+        <v>132.04999999999998</v>
+      </c>
+      <c r="F10" s="103"/>
       <c r="G10" s="89">
         <v>126</v>
       </c>
-      <c r="H10" s="105">
+      <c r="H10" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I10" s="73">
         <f t="shared" si="13"/>
-        <v>312.88249999999999</v>
+        <v>343.20649999999995</v>
       </c>
       <c r="J10" s="53"/>
       <c r="K10" s="53">
         <f t="shared" si="1"/>
-        <v>21.901775000000001</v>
+        <v>24.024455</v>
       </c>
       <c r="L10" s="53">
         <f t="shared" si="2"/>
-        <v>43.803550000000001</v>
+        <v>48.048909999999999</v>
       </c>
       <c r="M10" s="53">
         <f t="shared" si="3"/>
-        <v>65.705325000000002</v>
+        <v>72.073364999999995</v>
       </c>
       <c r="N10" s="53">
         <f t="shared" si="4"/>
-        <v>87.607100000000003</v>
+        <v>96.097819999999999</v>
       </c>
       <c r="O10" s="53">
         <f t="shared" si="5"/>
-        <v>109.508875</v>
+        <v>120.12227499999999</v>
       </c>
       <c r="P10" s="53">
         <f t="shared" si="6"/>
-        <v>131.41065</v>
+        <v>144.14672999999999</v>
       </c>
       <c r="Q10" s="53">
         <f t="shared" si="7"/>
-        <v>153.31242500000002</v>
+        <v>168.17118499999998</v>
       </c>
       <c r="R10" s="53">
         <f t="shared" si="8"/>
-        <v>175.21420000000001</v>
+        <v>192.19564</v>
       </c>
       <c r="S10" s="53">
         <f t="shared" si="9"/>
-        <v>197.11597500000002</v>
+        <v>216.22009500000001</v>
       </c>
       <c r="T10" s="53">
         <f t="shared" si="10"/>
-        <v>219.01775000000001</v>
+        <v>240.24454999999998</v>
       </c>
       <c r="U10" s="54">
         <f t="shared" si="11"/>
-        <v>240.91952499999999</v>
+        <v>264.26900499999999</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
@@ -1864,66 +1864,66 @@
       <c r="D11" s="63">
         <v>106</v>
       </c>
-      <c r="E11" s="98">
+      <c r="E11" s="103">
         <f t="shared" si="12"/>
-        <v>121.89999999999999</v>
-      </c>
-      <c r="F11" s="98"/>
+        <v>147.34</v>
+      </c>
+      <c r="F11" s="103"/>
       <c r="G11" s="89">
         <v>118</v>
       </c>
-      <c r="H11" s="105">
+      <c r="H11" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I11" s="73">
         <f t="shared" si="13"/>
-        <v>319.06700000000001</v>
+        <v>352.90220000000005</v>
       </c>
       <c r="J11" s="53"/>
       <c r="K11" s="53">
         <f t="shared" si="1"/>
-        <v>22.334690000000002</v>
+        <v>24.703154000000005</v>
       </c>
       <c r="L11" s="53">
         <f t="shared" si="2"/>
-        <v>44.669380000000004</v>
+        <v>49.40630800000001</v>
       </c>
       <c r="M11" s="53">
         <f t="shared" si="3"/>
-        <v>67.004070000000013</v>
+        <v>74.109462000000022</v>
       </c>
       <c r="N11" s="53">
         <f t="shared" si="4"/>
-        <v>89.338760000000008</v>
+        <v>98.81261600000002</v>
       </c>
       <c r="O11" s="53">
         <f t="shared" si="5"/>
-        <v>111.67345000000002</v>
+        <v>123.51577000000003</v>
       </c>
       <c r="P11" s="53">
         <f t="shared" si="6"/>
-        <v>134.00814000000003</v>
+        <v>148.21892400000004</v>
       </c>
       <c r="Q11" s="53">
         <f t="shared" si="7"/>
-        <v>156.34283000000002</v>
+        <v>172.92207800000003</v>
       </c>
       <c r="R11" s="53">
         <f t="shared" si="8"/>
-        <v>178.67752000000002</v>
+        <v>197.62523200000004</v>
       </c>
       <c r="S11" s="53">
         <f t="shared" si="9"/>
-        <v>201.01221000000004</v>
+        <v>222.32838600000008</v>
       </c>
       <c r="T11" s="53">
         <f t="shared" si="10"/>
-        <v>223.34690000000003</v>
+        <v>247.03154000000006</v>
       </c>
       <c r="U11" s="54">
         <f t="shared" si="11"/>
-        <v>245.68159</v>
+        <v>271.73469400000005</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
@@ -1937,66 +1937,66 @@
       <c r="D12" s="63">
         <v>111</v>
       </c>
-      <c r="E12" s="98">
+      <c r="E12" s="103">
         <f t="shared" si="12"/>
-        <v>127.64999999999999</v>
-      </c>
-      <c r="F12" s="98"/>
+        <v>154.29</v>
+      </c>
+      <c r="F12" s="103"/>
       <c r="G12" s="89">
         <v>118</v>
       </c>
-      <c r="H12" s="105">
+      <c r="H12" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I12" s="73">
         <f t="shared" si="13"/>
-        <v>326.71449999999999</v>
+        <v>362.14569999999998</v>
       </c>
       <c r="J12" s="53"/>
       <c r="K12" s="53">
         <f t="shared" si="1"/>
-        <v>22.870015000000002</v>
+        <v>25.350199</v>
       </c>
       <c r="L12" s="53">
         <f t="shared" si="2"/>
-        <v>45.740030000000004</v>
+        <v>50.700398</v>
       </c>
       <c r="M12" s="53">
         <f t="shared" si="3"/>
-        <v>68.610045</v>
+        <v>76.050596999999996</v>
       </c>
       <c r="N12" s="53">
         <f t="shared" si="4"/>
-        <v>91.480060000000009</v>
+        <v>101.400796</v>
       </c>
       <c r="O12" s="53">
         <f t="shared" si="5"/>
-        <v>114.350075</v>
+        <v>126.750995</v>
       </c>
       <c r="P12" s="53">
         <f t="shared" si="6"/>
-        <v>137.22009</v>
+        <v>152.10119399999999</v>
       </c>
       <c r="Q12" s="53">
         <f t="shared" si="7"/>
-        <v>160.09010500000002</v>
+        <v>177.451393</v>
       </c>
       <c r="R12" s="53">
         <f t="shared" si="8"/>
-        <v>182.96012000000002</v>
+        <v>202.801592</v>
       </c>
       <c r="S12" s="53">
         <f t="shared" si="9"/>
-        <v>205.83013500000004</v>
+        <v>228.15179100000003</v>
       </c>
       <c r="T12" s="53">
         <f t="shared" si="10"/>
-        <v>228.70015000000001</v>
+        <v>253.50199000000001</v>
       </c>
       <c r="U12" s="54">
         <f t="shared" si="11"/>
-        <v>251.570165</v>
+        <v>278.85218900000001</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
@@ -2012,66 +2012,66 @@
       <c r="D13" s="63">
         <v>111</v>
       </c>
-      <c r="E13" s="98">
+      <c r="E13" s="103">
         <f t="shared" si="12"/>
-        <v>127.64999999999999</v>
-      </c>
-      <c r="F13" s="98"/>
+        <v>154.29</v>
+      </c>
+      <c r="F13" s="103"/>
       <c r="G13" s="89">
         <v>128</v>
       </c>
-      <c r="H13" s="105">
+      <c r="H13" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I13" s="73">
         <f t="shared" si="13"/>
-        <v>340.0145</v>
+        <v>375.44569999999999</v>
       </c>
       <c r="J13" s="53"/>
       <c r="K13" s="53">
         <f t="shared" si="1"/>
-        <v>23.801015000000003</v>
+        <v>26.281199000000001</v>
       </c>
       <c r="L13" s="53">
         <f t="shared" si="2"/>
-        <v>47.602030000000006</v>
+        <v>52.562398000000002</v>
       </c>
       <c r="M13" s="53">
         <f t="shared" si="3"/>
-        <v>71.403045000000006</v>
+        <v>78.843597000000003</v>
       </c>
       <c r="N13" s="53">
         <f t="shared" si="4"/>
-        <v>95.204060000000013</v>
+        <v>105.124796</v>
       </c>
       <c r="O13" s="53">
         <f t="shared" si="5"/>
-        <v>119.00507500000001</v>
+        <v>131.40599500000002</v>
       </c>
       <c r="P13" s="53">
         <f t="shared" si="6"/>
-        <v>142.80609000000001</v>
+        <v>157.68719400000001</v>
       </c>
       <c r="Q13" s="53">
         <f t="shared" si="7"/>
-        <v>166.60710500000002</v>
+        <v>183.96839300000002</v>
       </c>
       <c r="R13" s="53">
         <f t="shared" si="8"/>
-        <v>190.40812000000003</v>
+        <v>210.24959200000001</v>
       </c>
       <c r="S13" s="53">
         <f t="shared" si="9"/>
-        <v>214.20913500000003</v>
+        <v>236.53079100000002</v>
       </c>
       <c r="T13" s="53">
         <f t="shared" si="10"/>
-        <v>238.01015000000001</v>
+        <v>262.81199000000004</v>
       </c>
       <c r="U13" s="54">
         <f t="shared" si="11"/>
-        <v>261.81116500000002</v>
+        <v>289.093189</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
@@ -2087,66 +2087,66 @@
       <c r="D14" s="63">
         <v>110</v>
       </c>
-      <c r="E14" s="98">
+      <c r="E14" s="103">
         <f t="shared" si="12"/>
-        <v>126.49999999999999</v>
-      </c>
-      <c r="F14" s="98"/>
+        <v>152.89999999999998</v>
+      </c>
+      <c r="F14" s="103"/>
       <c r="G14" s="89">
         <v>131</v>
       </c>
-      <c r="H14" s="105">
+      <c r="H14" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I14" s="73">
         <f t="shared" si="13"/>
-        <v>342.47500000000002</v>
+        <v>377.58699999999999</v>
       </c>
       <c r="J14" s="53"/>
       <c r="K14" s="53">
         <f t="shared" si="1"/>
-        <v>23.973250000000004</v>
+        <v>26.431090000000001</v>
       </c>
       <c r="L14" s="53">
         <f t="shared" si="2"/>
-        <v>47.946500000000007</v>
+        <v>52.862180000000002</v>
       </c>
       <c r="M14" s="53">
         <f t="shared" si="3"/>
-        <v>71.919750000000008</v>
+        <v>79.293270000000007</v>
       </c>
       <c r="N14" s="53">
         <f t="shared" si="4"/>
-        <v>95.893000000000015</v>
+        <v>105.72436</v>
       </c>
       <c r="O14" s="53">
         <f t="shared" si="5"/>
-        <v>119.86625000000002</v>
+        <v>132.15545</v>
       </c>
       <c r="P14" s="53">
         <f t="shared" si="6"/>
-        <v>143.83950000000002</v>
+        <v>158.58654000000001</v>
       </c>
       <c r="Q14" s="53">
         <f t="shared" si="7"/>
-        <v>167.81275000000002</v>
+        <v>185.01763000000003</v>
       </c>
       <c r="R14" s="53">
         <f t="shared" si="8"/>
-        <v>191.78600000000003</v>
+        <v>211.44872000000001</v>
       </c>
       <c r="S14" s="53">
         <f t="shared" si="9"/>
-        <v>215.75925000000007</v>
+        <v>237.87981000000005</v>
       </c>
       <c r="T14" s="53">
         <f t="shared" si="10"/>
-        <v>239.73250000000004</v>
+        <v>264.3109</v>
       </c>
       <c r="U14" s="54">
         <f t="shared" si="11"/>
-        <v>263.70575000000002</v>
+        <v>290.74198999999999</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="29" x14ac:dyDescent="0.35">
@@ -2160,66 +2160,66 @@
       <c r="D15" s="63">
         <v>99</v>
       </c>
-      <c r="E15" s="98">
+      <c r="E15" s="103">
         <f t="shared" si="12"/>
-        <v>113.85</v>
-      </c>
-      <c r="F15" s="98"/>
+        <v>137.60999999999999</v>
+      </c>
+      <c r="F15" s="103"/>
       <c r="G15" s="89">
         <v>100</v>
       </c>
-      <c r="H15" s="105">
+      <c r="H15" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I15" s="73">
         <f t="shared" si="13"/>
-        <v>284.4205</v>
+        <v>316.0213</v>
       </c>
       <c r="J15" s="53"/>
       <c r="K15" s="53">
         <f t="shared" si="1"/>
-        <v>19.909435000000002</v>
+        <v>22.121491000000002</v>
       </c>
       <c r="L15" s="53">
         <f t="shared" si="2"/>
-        <v>39.818870000000004</v>
+        <v>44.242982000000005</v>
       </c>
       <c r="M15" s="53">
         <f t="shared" si="3"/>
-        <v>59.728305000000006</v>
+        <v>66.364473000000004</v>
       </c>
       <c r="N15" s="53">
         <f t="shared" si="4"/>
-        <v>79.637740000000008</v>
+        <v>88.48596400000001</v>
       </c>
       <c r="O15" s="53">
         <f t="shared" si="5"/>
-        <v>99.54717500000001</v>
+        <v>110.60745500000002</v>
       </c>
       <c r="P15" s="53">
         <f t="shared" si="6"/>
-        <v>119.45661000000001</v>
+        <v>132.72894600000001</v>
       </c>
       <c r="Q15" s="53">
         <f t="shared" si="7"/>
-        <v>139.36604500000001</v>
+        <v>154.850437</v>
       </c>
       <c r="R15" s="53">
         <f t="shared" si="8"/>
-        <v>159.27548000000002</v>
+        <v>176.97192800000002</v>
       </c>
       <c r="S15" s="53">
         <f t="shared" si="9"/>
-        <v>179.18491500000005</v>
+        <v>199.09341900000004</v>
       </c>
       <c r="T15" s="53">
         <f t="shared" si="10"/>
-        <v>199.09435000000002</v>
+        <v>221.21491000000003</v>
       </c>
       <c r="U15" s="54">
         <f t="shared" si="11"/>
-        <v>219.00378500000002</v>
+        <v>243.336401</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
@@ -2235,66 +2235,66 @@
       <c r="D16" s="63">
         <v>108</v>
       </c>
-      <c r="E16" s="98">
+      <c r="E16" s="103">
         <f t="shared" si="12"/>
-        <v>124.19999999999999</v>
-      </c>
-      <c r="F16" s="98"/>
+        <v>150.11999999999998</v>
+      </c>
+      <c r="F16" s="103"/>
       <c r="G16" s="89">
         <v>100</v>
       </c>
-      <c r="H16" s="105">
+      <c r="H16" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I16" s="73">
         <f t="shared" si="13"/>
-        <v>298.18599999999998</v>
+        <v>332.65960000000001</v>
       </c>
       <c r="J16" s="53"/>
       <c r="K16" s="53">
         <f t="shared" si="1"/>
-        <v>20.87302</v>
+        <v>23.286172000000004</v>
       </c>
       <c r="L16" s="53">
         <f t="shared" si="2"/>
-        <v>41.746040000000001</v>
+        <v>46.572344000000008</v>
       </c>
       <c r="M16" s="53">
         <f t="shared" si="3"/>
-        <v>62.619060000000005</v>
+        <v>69.858516000000009</v>
       </c>
       <c r="N16" s="53">
         <f t="shared" si="4"/>
-        <v>83.492080000000001</v>
+        <v>93.144688000000016</v>
       </c>
       <c r="O16" s="53">
         <f t="shared" si="5"/>
-        <v>104.3651</v>
+        <v>116.43086000000001</v>
       </c>
       <c r="P16" s="53">
         <f t="shared" si="6"/>
-        <v>125.23812000000001</v>
+        <v>139.71703200000002</v>
       </c>
       <c r="Q16" s="53">
         <f t="shared" si="7"/>
-        <v>146.11114000000001</v>
+        <v>163.00320400000001</v>
       </c>
       <c r="R16" s="53">
         <f t="shared" si="8"/>
-        <v>166.98416</v>
+        <v>186.28937600000003</v>
       </c>
       <c r="S16" s="53">
         <f t="shared" si="9"/>
-        <v>187.85718000000003</v>
+        <v>209.57554800000005</v>
       </c>
       <c r="T16" s="53">
         <f t="shared" si="10"/>
-        <v>208.7302</v>
+        <v>232.86172000000002</v>
       </c>
       <c r="U16" s="54">
         <f t="shared" si="11"/>
-        <v>229.60321999999999</v>
+        <v>256.14789200000001</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
@@ -2310,66 +2310,66 @@
       <c r="D17" s="63">
         <v>105</v>
       </c>
-      <c r="E17" s="98">
+      <c r="E17" s="103">
         <f t="shared" si="12"/>
-        <v>120.74999999999999</v>
-      </c>
-      <c r="F17" s="98"/>
+        <v>145.94999999999999</v>
+      </c>
+      <c r="F17" s="103"/>
       <c r="G17" s="89">
         <v>122</v>
       </c>
-      <c r="H17" s="105">
+      <c r="H17" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I17" s="73">
         <f t="shared" si="13"/>
-        <v>322.85750000000002</v>
+        <v>356.37349999999998</v>
       </c>
       <c r="J17" s="53"/>
       <c r="K17" s="53">
         <f t="shared" si="1"/>
-        <v>22.600025000000002</v>
+        <v>24.946145000000001</v>
       </c>
       <c r="L17" s="53">
         <f t="shared" si="2"/>
-        <v>45.200050000000005</v>
+        <v>49.892290000000003</v>
       </c>
       <c r="M17" s="53">
         <f t="shared" si="3"/>
-        <v>67.800075000000007</v>
+        <v>74.838435000000004</v>
       </c>
       <c r="N17" s="53">
         <f t="shared" si="4"/>
-        <v>90.400100000000009</v>
+        <v>99.784580000000005</v>
       </c>
       <c r="O17" s="53">
         <f t="shared" si="5"/>
-        <v>113.00012500000001</v>
+        <v>124.73072500000001</v>
       </c>
       <c r="P17" s="53">
         <f t="shared" si="6"/>
-        <v>135.60015000000001</v>
+        <v>149.67687000000001</v>
       </c>
       <c r="Q17" s="53">
         <f t="shared" si="7"/>
-        <v>158.20017500000003</v>
+        <v>174.62301500000001</v>
       </c>
       <c r="R17" s="53">
         <f t="shared" si="8"/>
-        <v>180.80020000000002</v>
+        <v>199.56916000000001</v>
       </c>
       <c r="S17" s="53">
         <f t="shared" si="9"/>
-        <v>203.40022500000003</v>
+        <v>224.51530500000004</v>
       </c>
       <c r="T17" s="53">
         <f t="shared" si="10"/>
-        <v>226.00025000000002</v>
+        <v>249.46145000000001</v>
       </c>
       <c r="U17" s="54">
         <f t="shared" si="11"/>
-        <v>248.60027500000001</v>
+        <v>274.40759500000001</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
@@ -2385,66 +2385,66 @@
       <c r="D18" s="63">
         <v>97</v>
       </c>
-      <c r="E18" s="98">
+      <c r="E18" s="103">
         <f t="shared" si="12"/>
-        <v>111.55</v>
-      </c>
-      <c r="F18" s="98"/>
+        <v>134.82999999999998</v>
+      </c>
+      <c r="F18" s="103"/>
       <c r="G18" s="89">
         <v>88</v>
       </c>
-      <c r="H18" s="105">
+      <c r="H18" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I18" s="73">
         <f t="shared" si="13"/>
-        <v>265.40150000000006</v>
+        <v>296.3639</v>
       </c>
       <c r="J18" s="53"/>
       <c r="K18" s="53">
         <f t="shared" si="1"/>
-        <v>18.578105000000004</v>
+        <v>20.745473</v>
       </c>
       <c r="L18" s="53">
         <f t="shared" si="2"/>
-        <v>37.156210000000009</v>
+        <v>41.490946000000001</v>
       </c>
       <c r="M18" s="53">
         <f t="shared" si="3"/>
-        <v>55.734315000000016</v>
+        <v>62.236419000000005</v>
       </c>
       <c r="N18" s="53">
         <f t="shared" si="4"/>
-        <v>74.312420000000017</v>
+        <v>82.981892000000002</v>
       </c>
       <c r="O18" s="53">
         <f t="shared" si="5"/>
-        <v>92.890525000000025</v>
+        <v>103.72736500000001</v>
       </c>
       <c r="P18" s="53">
         <f t="shared" si="6"/>
-        <v>111.46863000000003</v>
+        <v>124.47283800000001</v>
       </c>
       <c r="Q18" s="53">
         <f t="shared" si="7"/>
-        <v>130.04673500000004</v>
+        <v>145.21831100000003</v>
       </c>
       <c r="R18" s="53">
         <f t="shared" si="8"/>
-        <v>148.62484000000003</v>
+        <v>165.963784</v>
       </c>
       <c r="S18" s="53">
         <f t="shared" si="9"/>
-        <v>167.20294500000006</v>
+        <v>186.70925700000004</v>
       </c>
       <c r="T18" s="53">
         <f t="shared" si="10"/>
-        <v>185.78105000000005</v>
+        <v>207.45473000000001</v>
       </c>
       <c r="U18" s="54">
         <f t="shared" si="11"/>
-        <v>204.35915500000004</v>
+        <v>228.20020300000002</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="29" x14ac:dyDescent="0.35">
@@ -2460,66 +2460,66 @@
       <c r="D19" s="63">
         <v>106</v>
       </c>
-      <c r="E19" s="98">
+      <c r="E19" s="103">
         <f t="shared" si="12"/>
-        <v>121.89999999999999</v>
-      </c>
-      <c r="F19" s="98"/>
+        <v>147.34</v>
+      </c>
+      <c r="F19" s="103"/>
       <c r="G19" s="89">
         <v>85</v>
       </c>
-      <c r="H19" s="105">
+      <c r="H19" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I19" s="73">
         <f t="shared" si="13"/>
-        <v>275.17699999999996</v>
+        <v>309.01220000000001</v>
       </c>
       <c r="J19" s="53"/>
       <c r="K19" s="53">
         <f t="shared" si="1"/>
-        <v>19.26239</v>
+        <v>21.630854000000003</v>
       </c>
       <c r="L19" s="53">
         <f t="shared" si="2"/>
-        <v>38.52478</v>
+        <v>43.261708000000006</v>
       </c>
       <c r="M19" s="53">
         <f t="shared" si="3"/>
-        <v>57.787169999999996</v>
+        <v>64.892562000000012</v>
       </c>
       <c r="N19" s="53">
         <f t="shared" si="4"/>
-        <v>77.04956</v>
+        <v>86.523416000000012</v>
       </c>
       <c r="O19" s="53">
         <f t="shared" si="5"/>
-        <v>96.311949999999996</v>
+        <v>108.15427000000001</v>
       </c>
       <c r="P19" s="53">
         <f t="shared" si="6"/>
-        <v>115.57433999999999</v>
+        <v>129.78512400000002</v>
       </c>
       <c r="Q19" s="53">
         <f t="shared" si="7"/>
-        <v>134.83672999999999</v>
+        <v>151.41597800000002</v>
       </c>
       <c r="R19" s="53">
         <f t="shared" si="8"/>
-        <v>154.09912</v>
+        <v>173.04683200000002</v>
       </c>
       <c r="S19" s="53">
         <f t="shared" si="9"/>
-        <v>173.36151000000001</v>
+        <v>194.67768600000005</v>
       </c>
       <c r="T19" s="53">
         <f t="shared" si="10"/>
-        <v>192.62389999999999</v>
+        <v>216.30854000000002</v>
       </c>
       <c r="U19" s="54">
         <f t="shared" si="11"/>
-        <v>211.88628999999997</v>
+        <v>237.93939400000002</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
@@ -2533,66 +2533,66 @@
       <c r="D20" s="63">
         <v>98</v>
       </c>
-      <c r="E20" s="98">
+      <c r="E20" s="103">
         <f t="shared" si="12"/>
-        <v>112.69999999999999</v>
-      </c>
-      <c r="F20" s="98"/>
+        <v>136.22</v>
+      </c>
+      <c r="F20" s="103"/>
       <c r="G20" s="89">
         <v>85</v>
       </c>
-      <c r="H20" s="105">
+      <c r="H20" s="98">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I20" s="73">
         <f t="shared" si="13"/>
-        <v>262.94099999999997</v>
+        <v>294.2226</v>
       </c>
       <c r="J20" s="53"/>
       <c r="K20" s="53">
         <f t="shared" si="1"/>
-        <v>18.40587</v>
+        <v>20.595582</v>
       </c>
       <c r="L20" s="53">
         <f t="shared" si="2"/>
-        <v>36.81174</v>
+        <v>41.191164000000001</v>
       </c>
       <c r="M20" s="53">
         <f t="shared" si="3"/>
-        <v>55.217610000000001</v>
+        <v>61.786746000000008</v>
       </c>
       <c r="N20" s="53">
         <f t="shared" si="4"/>
-        <v>73.623480000000001</v>
+        <v>82.382328000000001</v>
       </c>
       <c r="O20" s="53">
         <f t="shared" si="5"/>
-        <v>92.029349999999994</v>
+        <v>102.97791000000001</v>
       </c>
       <c r="P20" s="53">
         <f t="shared" si="6"/>
-        <v>110.43522</v>
+        <v>123.57349200000002</v>
       </c>
       <c r="Q20" s="53">
         <f t="shared" si="7"/>
-        <v>128.84109000000001</v>
+        <v>144.16907400000002</v>
       </c>
       <c r="R20" s="53">
         <f t="shared" si="8"/>
-        <v>147.24696</v>
+        <v>164.764656</v>
       </c>
       <c r="S20" s="53">
         <f t="shared" si="9"/>
-        <v>165.65283000000002</v>
+        <v>185.36023800000004</v>
       </c>
       <c r="T20" s="53">
         <f t="shared" si="10"/>
-        <v>184.05869999999999</v>
+        <v>205.95582000000002</v>
       </c>
       <c r="U20" s="54">
         <f t="shared" si="11"/>
-        <v>202.46456999999998</v>
+        <v>226.551402</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2606,66 +2606,66 @@
       <c r="D21" s="77">
         <v>87</v>
       </c>
-      <c r="E21" s="102">
+      <c r="E21" s="104">
         <f t="shared" si="12"/>
-        <v>100.05</v>
-      </c>
-      <c r="F21" s="102"/>
+        <v>120.92999999999999</v>
+      </c>
+      <c r="F21" s="104"/>
       <c r="G21" s="90">
         <v>0</v>
       </c>
-      <c r="H21" s="106">
+      <c r="H21" s="99">
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
       <c r="I21" s="78">
         <f t="shared" si="13"/>
-        <v>133.06649999999999</v>
+        <v>160.83689999999999</v>
       </c>
       <c r="J21" s="55"/>
       <c r="K21" s="55">
         <f t="shared" si="1"/>
-        <v>9.3146550000000001</v>
+        <v>11.258583</v>
       </c>
       <c r="L21" s="55">
         <f t="shared" si="2"/>
-        <v>18.62931</v>
+        <v>22.517166</v>
       </c>
       <c r="M21" s="55">
         <f t="shared" si="3"/>
-        <v>27.943965000000002</v>
+        <v>33.775748999999998</v>
       </c>
       <c r="N21" s="55">
         <f t="shared" si="4"/>
-        <v>37.258620000000001</v>
+        <v>45.034331999999999</v>
       </c>
       <c r="O21" s="55">
         <f t="shared" si="5"/>
-        <v>46.573275000000002</v>
+        <v>56.292915000000001</v>
       </c>
       <c r="P21" s="55">
         <f t="shared" si="6"/>
-        <v>55.887930000000004</v>
+        <v>67.551497999999995</v>
       </c>
       <c r="Q21" s="55">
         <f t="shared" si="7"/>
-        <v>65.202584999999999</v>
+        <v>78.810080999999997</v>
       </c>
       <c r="R21" s="55">
         <f t="shared" si="8"/>
-        <v>74.517240000000001</v>
+        <v>90.068663999999998</v>
       </c>
       <c r="S21" s="55">
         <f t="shared" si="9"/>
-        <v>83.831895000000003</v>
+        <v>101.32724700000001</v>
       </c>
       <c r="T21" s="55">
         <f t="shared" si="10"/>
-        <v>93.146550000000005</v>
+        <v>112.58583</v>
       </c>
       <c r="U21" s="56">
         <f t="shared" si="11"/>
-        <v>102.46120499999999</v>
+        <v>123.84441299999999</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
@@ -2679,7 +2679,7 @@
       <c r="E24" s="35"/>
       <c r="F24" s="35"/>
       <c r="G24" s="36"/>
-      <c r="H24" s="108"/>
+      <c r="H24" s="101"/>
       <c r="I24" s="29" t="s">
         <v>26</v>
       </c>
@@ -3206,7 +3206,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="109"/>
+      <c r="H34" s="102"/>
       <c r="I34" s="23">
         <v>250</v>
       </c>
@@ -4220,6 +4220,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E5:F5"/>
@@ -4236,11 +4241,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <conditionalFormatting sqref="K4:U21">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">

</xml_diff>